<commit_message>
Update 2020180047 권세진 졸업작품 계획표.xlsx
</commit_message>
<xml_diff>
--- a/졸업작품 제안서/2020180047 권세진 졸업작품 계획표.xlsx
+++ b/졸업작품 제안서/2020180047 권세진 졸업작품 계획표.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sejin\Downloads\GraduationWork\졸업작품 제안서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404675FE-C588-4CC7-B6E7-DF76528E9334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9154CACB-2C90-4E9D-B2E0-0816C3A95175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C4D6BBA-0759-4F1A-B9D9-1B1D459706EC}"/>
   </bookViews>
@@ -226,24 +226,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서버 모델 정하기 및 서버에서만 실행되어야 할 기능들 프로토타입 형식으로 구현해보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>졸업작품에서 쓰일 서버 모델을 통해 서버 구축</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>졸업작품에서 쓰일 서버 모델을 통해 
 서버 구축 시작하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">9월 미완 계획 보충 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>12월 1주차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버 모델 정하기 및 네트워크 통신 공부
+클라이언트와 iocp 소켓 입출력 공부
+언리얼 네트워크 통신 기능 공부를 통한 iocp 연동 공부 (FSocket 등등)
+언리얼 iocp 활용 예제 코드 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9월 미완 계획 보충 
+서버에서만 사용할 기능들 구현해보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">졸업작품에서 쓰일 서버 모델을 통해 서버 구축
+및 클라이언트 연동하기(패킷연동) </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -999,7 +1004,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1012,6 +1017,234 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1039,15 +1272,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,12 +1279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1069,239 +1287,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1620,7 +1628,7 @@
   <dimension ref="A8:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36:K38"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1634,671 +1642,654 @@
   <sheetData>
     <row r="8" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="30"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="68"/>
     </row>
     <row r="10" spans="1:19" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="33"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="71"/>
     </row>
     <row r="11" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="40" t="s">
+      <c r="E11" s="75"/>
+      <c r="F11" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="40" t="s">
+      <c r="G11" s="77"/>
+      <c r="H11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="41"/>
-      <c r="J11" s="40" t="s">
+      <c r="I11" s="77"/>
+      <c r="J11" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="34" t="s">
+      <c r="K11" s="77"/>
+      <c r="L11" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="42"/>
-      <c r="N11" s="34" t="s">
+      <c r="M11" s="78"/>
+      <c r="N11" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="35" t="s">
+      <c r="O11" s="21"/>
+      <c r="P11" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="34" t="s">
+      <c r="Q11" s="21"/>
+      <c r="R11" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="S11" s="36"/>
+      <c r="S11" s="73"/>
     </row>
     <row r="12" spans="1:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="51" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46" t="s">
+      <c r="I12" s="57"/>
+      <c r="J12" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="54" t="s">
+      <c r="K12" s="96"/>
+      <c r="L12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="4" t="s">
+      <c r="M12" s="54"/>
+      <c r="N12" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="6"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="82"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
+      <c r="S13" s="85"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="59"/>
+      <c r="D14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="13" t="s">
+      <c r="E14" s="59"/>
+      <c r="F14" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="59"/>
+      <c r="H14" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="21" t="s">
+      <c r="I14" s="59"/>
+      <c r="J14" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="19" t="s">
+      <c r="K14" s="93"/>
+      <c r="L14" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19" t="s">
+      <c r="M14" s="55"/>
+      <c r="N14" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="20"/>
-      <c r="P14" s="19" t="s">
+      <c r="O14" s="54"/>
+      <c r="P14" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="19" t="s">
+      <c r="Q14" s="54"/>
+      <c r="R14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="S14" s="20"/>
+      <c r="S14" s="54"/>
     </row>
     <row r="15" spans="1:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="13"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="54"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="61"/>
+      <c r="D16" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="52" t="s">
+      <c r="E16" s="61"/>
+      <c r="F16" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B17" s="23"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="23" t="s">
+      <c r="B17" s="63"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="61"/>
       <c r="H17" s="2"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B18" s="23"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="53" t="s">
+      <c r="B18" s="63"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="61"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B19" s="23"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="26"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B20" s="24"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="27"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="12"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+      <c r="O21" s="87"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="87"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="88"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="15"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="59"/>
     </row>
     <row r="23" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="18"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
+      <c r="O23" s="90"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="90"/>
+      <c r="S23" s="91"/>
     </row>
     <row r="24" spans="2:19" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="57"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="49"/>
     </row>
     <row r="26" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="58"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="59"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="51"/>
     </row>
     <row r="27" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="60" t="s">
+      <c r="C27" s="52"/>
+      <c r="D27" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="61"/>
-      <c r="F27" s="60" t="s">
+      <c r="E27" s="52"/>
+      <c r="F27" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="61"/>
-      <c r="H27" s="60" t="s">
+      <c r="G27" s="52"/>
+      <c r="H27" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="60" t="s">
+      <c r="I27" s="52"/>
+      <c r="J27" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="61"/>
-      <c r="L27" s="60" t="s">
+      <c r="K27" s="52"/>
+      <c r="L27" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="M27" s="61"/>
-      <c r="N27" s="60" t="s">
+      <c r="M27" s="52"/>
+      <c r="N27" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="O27" s="61"/>
-      <c r="P27" s="60" t="s">
+      <c r="O27" s="52"/>
+      <c r="P27" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="Q27" s="61"/>
+      <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="91" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="36"/>
+    </row>
+    <row r="29" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="39"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B30" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="O28" s="67"/>
-      <c r="P28" s="67"/>
-      <c r="Q28" s="68"/>
-    </row>
-    <row r="29" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="84"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="100"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="70"/>
-      <c r="P29" s="70"/>
-      <c r="Q29" s="71"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B30" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="93" t="s">
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="97"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="44"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="90"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="87"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="97"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="44"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B32" s="86"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="87"/>
-      <c r="P32" s="87"/>
-      <c r="Q32" s="97"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="44"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="87"/>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="97"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="44"/>
     </row>
     <row r="34" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="88"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="96"/>
-      <c r="L34" s="96"/>
-      <c r="M34" s="96"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="92"/>
-      <c r="Q34" s="98"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="46"/>
     </row>
     <row r="35" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44" t="s">
+      <c r="C35" s="41"/>
+      <c r="D35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44" t="s">
+      <c r="E35" s="41"/>
+      <c r="F35" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44" t="s">
+      <c r="G35" s="41"/>
+      <c r="H35" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="44"/>
-      <c r="J35" s="94" t="s">
+      <c r="I35" s="41"/>
+      <c r="J35" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" s="24"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="21"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B36" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K35" s="89"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B36" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="79" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="75"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B37" s="76"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="75"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="4"/>
     </row>
     <row r="38" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="83"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B36:E38"/>
-    <mergeCell ref="F36:K38"/>
-    <mergeCell ref="B28:I29"/>
-    <mergeCell ref="B30:I34"/>
-    <mergeCell ref="J30:M34"/>
-    <mergeCell ref="J28:M29"/>
-    <mergeCell ref="N28:Q29"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N30:Q34"/>
-    <mergeCell ref="B25:Q26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="N14:O20"/>
-    <mergeCell ref="P14:Q20"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="L21:S23"/>
+    <mergeCell ref="R14:S20"/>
+    <mergeCell ref="J14:K20"/>
+    <mergeCell ref="B16:C20"/>
+    <mergeCell ref="D16:E20"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="L14:M20"/>
+    <mergeCell ref="B21:K23"/>
+    <mergeCell ref="F14:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="F17:G17"/>
@@ -2314,18 +2305,35 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="B12:G13"/>
     <mergeCell ref="N12:S13"/>
-    <mergeCell ref="L21:S23"/>
-    <mergeCell ref="R14:S20"/>
-    <mergeCell ref="J14:K20"/>
-    <mergeCell ref="B16:C20"/>
-    <mergeCell ref="D16:E20"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="D14:E15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L14:M20"/>
     <mergeCell ref="J12:K13"/>
-    <mergeCell ref="B21:K23"/>
-    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="N14:O20"/>
+    <mergeCell ref="P14:Q20"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="B25:Q26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N28:Q29"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N30:Q34"/>
+    <mergeCell ref="B36:E38"/>
+    <mergeCell ref="F36:K38"/>
+    <mergeCell ref="B28:I29"/>
+    <mergeCell ref="B30:I34"/>
+    <mergeCell ref="J30:M34"/>
+    <mergeCell ref="J28:M29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>